<commit_message>
Solve Leetcode - 199. Binary Tree Right Side View
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{279D4840-EC92-484A-AE75-E73DBB348547}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E59563E0-6449-460C-8914-CDEA9779E74A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Problem Logs" sheetId="1" r:id="rId1"/>
+    <sheet name="Neetcode 150" sheetId="1" r:id="rId1"/>
     <sheet name="Extra" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -103,12 +103,24 @@
   <si>
     <t>The color of the dsa question name is the indicator of how hard it was for me personally</t>
   </si>
+  <si>
+    <t>102. Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t>Do a BFS. can do it with deque but since we have to store values at each level, use an auxilary array instead. Initialize buffer array with temp, while buffer_arr is true, iterate and add each child at this level and store it in a temp array (save values too separately), then replace buffer with temp and repeat</t>
+  </si>
+  <si>
+    <t>199. Binary Tree Right Side View</t>
+  </si>
+  <si>
+    <t>DFS and track level. Append if len(res) == level. Cause if res = [] and level = 0 (root) then this is the first node at that level so add node.val. This way res.length will grow and it'll make sure we don’t add another node for the same level</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +139,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,11 +174,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -171,9 +192,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -187,6 +210,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,11 +520,42 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EF84472B-74D8-4E9E-82AC-B98F09246ED6}"/>
+    <hyperlink ref="C4" r:id="rId2" display="https://leetcode.com/problems/binary-tree-right-side-view/" xr:uid="{A5201EEF-4843-450C-BB22-72FA29685321}"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://leetcode.com/problems/binary-tree-level-order-traversal/" xr:uid="{C0EB787D-94FE-4A31-A6E4-D67C2FC86C31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 1448. Count Good Nodes in Binary Tree - DFS
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E59563E0-6449-460C-8914-CDEA9779E74A}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3938C9E6-86DD-4694-AD00-1AD3E4A5555F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>DFS and track level. Append if len(res) == level. Cause if res = [] and level = 0 (root) then this is the first node at that level so add node.val. This way res.length will grow and it'll make sure we don’t add another node for the same level</t>
+  </si>
+  <si>
+    <t>Just iterate over it in dfs and keep track of the max value of all parents/ancestors of this node, if node.val &gt;= then we can add (and update max), otherwise continue dfs</t>
+  </si>
+  <si>
+    <t>1448. Count Good Nodes in Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -479,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,14 +554,29 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EF84472B-74D8-4E9E-82AC-B98F09246ED6}"/>
     <hyperlink ref="C4" r:id="rId2" display="https://leetcode.com/problems/binary-tree-right-side-view/" xr:uid="{A5201EEF-4843-450C-BB22-72FA29685321}"/>
     <hyperlink ref="C3" r:id="rId3" display="https://leetcode.com/problems/binary-tree-level-order-traversal/" xr:uid="{C0EB787D-94FE-4A31-A6E4-D67C2FC86C31}"/>
+    <hyperlink ref="C5" r:id="rId4" display="https://leetcode.com/problems/count-good-nodes-in-binary-tree/" xr:uid="{0FD1E5C2-E200-48B0-817A-FCE06967530C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 98. Validate Binary Search Tree - Inorder
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3938C9E6-86DD-4694-AD00-1AD3E4A5555F}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21D1851F-8F7D-4323-A4D4-986DA2097DA6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>1448. Count Good Nodes in Binary Tree</t>
+  </si>
+  <si>
+    <t>98. Validate Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Do inorder traversal and check if prev &lt; node.val, for each node otherwise return False. For it to be a binary tree, the inorder MUST be non-increasing/non-decreasing(or ascending/descending, depends on type of bst). Checking for node.left &lt; node.val &lt; node.right for each node is not enough</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -199,6 +205,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -485,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,15 +577,30 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EF84472B-74D8-4E9E-82AC-B98F09246ED6}"/>
     <hyperlink ref="C4" r:id="rId2" display="https://leetcode.com/problems/binary-tree-right-side-view/" xr:uid="{A5201EEF-4843-450C-BB22-72FA29685321}"/>
     <hyperlink ref="C3" r:id="rId3" display="https://leetcode.com/problems/binary-tree-level-order-traversal/" xr:uid="{C0EB787D-94FE-4A31-A6E4-D67C2FC86C31}"/>
     <hyperlink ref="C5" r:id="rId4" display="https://leetcode.com/problems/count-good-nodes-in-binary-tree/" xr:uid="{0FD1E5C2-E200-48B0-817A-FCE06967530C}"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://leetcode.com/problems/validate-binary-search-tree/" xr:uid="{91604824-7E59-4C2A-8FB8-0B65650BAEA2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 105. Construct Binary Tree from Preorder and Inorder Traversal - BFS style tree building
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21D1851F-8F7D-4323-A4D4-986DA2097DA6}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEE00793-2D27-4E2B-84F2-9EA2DE049809}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -127,12 +127,18 @@
   <si>
     <t>Do inorder traversal and check if prev &lt; node.val, for each node otherwise return False. For it to be a binary tree, the inorder MUST be non-increasing/non-decreasing(or ascending/descending, depends on type of bst). Checking for node.left &lt; node.val &lt; node.right for each node is not enough</t>
   </si>
+  <si>
+    <t>230. Kth Smallest Element in a BST</t>
+  </si>
+  <si>
+    <t>Inorder will give us the elements sorted in ascending order, just find the kth element there</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +165,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -204,10 +217,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -494,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,7 +555,7 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -584,20 +597,34 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EF84472B-74D8-4E9E-82AC-B98F09246ED6}"/>
     <hyperlink ref="C4" r:id="rId2" display="https://leetcode.com/problems/binary-tree-right-side-view/" xr:uid="{A5201EEF-4843-450C-BB22-72FA29685321}"/>
-    <hyperlink ref="C3" r:id="rId3" display="https://leetcode.com/problems/binary-tree-level-order-traversal/" xr:uid="{C0EB787D-94FE-4A31-A6E4-D67C2FC86C31}"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://leetcode.com/problems/count-good-nodes-in-binary-tree/" xr:uid="{0FD1E5C2-E200-48B0-817A-FCE06967530C}"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://leetcode.com/problems/validate-binary-search-tree/" xr:uid="{91604824-7E59-4C2A-8FB8-0B65650BAEA2}"/>
+    <hyperlink ref="C5" r:id="rId3" display="https://leetcode.com/problems/count-good-nodes-in-binary-tree/" xr:uid="{0FD1E5C2-E200-48B0-817A-FCE06967530C}"/>
+    <hyperlink ref="C6" r:id="rId4" display="https://leetcode.com/problems/validate-binary-search-tree/" xr:uid="{91604824-7E59-4C2A-8FB8-0B65650BAEA2}"/>
+    <hyperlink ref="C7" r:id="rId5" display="https://leetcode.com/problems/kth-smallest-element-in-a-bst/" xr:uid="{BC985D1B-C1C8-46C7-A4CB-631018511FEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
Solve Leetcode - 124. Binary Tree Maximum Path Sum
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEE00793-2D27-4E2B-84F2-9EA2DE049809}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BAB6506-D105-412D-B74E-8942AFCC9940}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -133,12 +133,22 @@
   <si>
     <t>Inorder will give us the elements sorted in ascending order, just find the kth element there</t>
   </si>
+  <si>
+    <t>105. Construct Binary Tree from Preorder and Inorder Traversal</t>
+  </si>
+  <si>
+    <t>Inorder gives left-to-right node order; preorder gives root-first traversal (root -&gt; left -&gt; right).
+Take preorder[0] as root. Find it in inorder, nodes left of it go to the left subtree, right go to the right subtree.
+Recurse on corresponding slices of preorder and inorder to build subtrees.
+Map inorder values to indices for O(1) lookups.
+Use DFS with start/end indices to control subtree bounds. If start == end, it's a leaf node.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,8 +186,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +204,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -199,12 +221,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -221,10 +244,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,6 +645,20 @@
         <v>21</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EF84472B-74D8-4E9E-82AC-B98F09246ED6}"/>
@@ -625,9 +666,10 @@
     <hyperlink ref="C5" r:id="rId3" display="https://leetcode.com/problems/count-good-nodes-in-binary-tree/" xr:uid="{0FD1E5C2-E200-48B0-817A-FCE06967530C}"/>
     <hyperlink ref="C6" r:id="rId4" display="https://leetcode.com/problems/validate-binary-search-tree/" xr:uid="{91604824-7E59-4C2A-8FB8-0B65650BAEA2}"/>
     <hyperlink ref="C7" r:id="rId5" display="https://leetcode.com/problems/kth-smallest-element-in-a-bst/" xr:uid="{BC985D1B-C1C8-46C7-A4CB-631018511FEF}"/>
+    <hyperlink ref="C8" r:id="rId6" display="https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/" xr:uid="{E6A98884-971B-40A3-AC5B-E52A1063EF44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 297. Serialize and Deserialize Binary Tree
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BAB6506-D105-412D-B74E-8942AFCC9940}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40362F01-8E08-4583-9F3E-8A8C67F8ECDC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -142,6 +142,16 @@
 Recurse on corresponding slices of preorder and inorder to build subtrees.
 Map inorder values to indices for O(1) lookups.
 Use DFS with start/end indices to control subtree bounds. If start == end, it's a leaf node.</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>124. Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t>We need to find the max path, so there can be only 1 straight path in the left subtree and right subtree
+So We'll do a post-order traversal because we need to find the maxPathSum for left and right subtree before we do calculations. And on each node of the subtrees, we have to add the max among the 3 choices, node.val itself, node.val + maxPathSum(left subtree) or node.val + maxPathSum(right subtree). Another Special case we need to consider is that the maxPath may not go through the root, it could go through any node, and thats what self.max_max will track, it'll track the max if the max path was passing through the current node from left to right (not up)</t>
   </si>
 </sst>
 </file>
@@ -227,7 +237,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -244,8 +254,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -534,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,11 +663,25 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -667,9 +692,10 @@
     <hyperlink ref="C6" r:id="rId4" display="https://leetcode.com/problems/validate-binary-search-tree/" xr:uid="{91604824-7E59-4C2A-8FB8-0B65650BAEA2}"/>
     <hyperlink ref="C7" r:id="rId5" display="https://leetcode.com/problems/kth-smallest-element-in-a-bst/" xr:uid="{BC985D1B-C1C8-46C7-A4CB-631018511FEF}"/>
     <hyperlink ref="C8" r:id="rId6" display="https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/" xr:uid="{E6A98884-971B-40A3-AC5B-E52A1063EF44}"/>
+    <hyperlink ref="C9" r:id="rId7" display="https://leetcode.com/problems/binary-tree-maximum-path-sum/" xr:uid="{21A06B24-7F83-4F58-A5DA-60FC2BE88869}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 973. K Closest Points to Origin - In Place Quick Select (Hoare)
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40362F01-8E08-4583-9F3E-8A8C67F8ECDC}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B5AA428-D433-4950-AF22-A6366D3077A7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -152,6 +152,30 @@
   <si>
     <t>We need to find the max path, so there can be only 1 straight path in the left subtree and right subtree
 So We'll do a post-order traversal because we need to find the maxPathSum for left and right subtree before we do calculations. And on each node of the subtrees, we have to add the max among the 3 choices, node.val itself, node.val + maxPathSum(left subtree) or node.val + maxPathSum(right subtree). Another Special case we need to consider is that the maxPath may not go through the root, it could go through any node, and thats what self.max_max will track, it'll track the max if the max path was passing through the current node from left to right (not up)</t>
+  </si>
+  <si>
+    <t>297. Serialize and Deserialize Binary Tree</t>
+  </si>
+  <si>
+    <t>First serialize into an array using preorder traversal and then return it as string with ",".join(serialized). Next split the serialized over "," and iterate over values (maybe store the vals into an iterator with vals = iter(data) and rebuild the same way you serialized using preorder</t>
+  </si>
+  <si>
+    <t>Heap/PQ</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>703. Kth Largest Element in a Stream</t>
+  </si>
+  <si>
+    <t>Use a heap to track top k elements (remove any elements after k for optmization)</t>
+  </si>
+  <si>
+    <t>1046. Last Stone Weight</t>
+  </si>
+  <si>
+    <t>Just use a heap. Re add elements to the heap again after using them (if needed). Be careful with the negatives since python max heap needs you to flip the signs</t>
   </si>
 </sst>
 </file>
@@ -545,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,6 +708,48 @@
         <v>26</v>
       </c>
     </row>
+    <row r="10" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EF84472B-74D8-4E9E-82AC-B98F09246ED6}"/>
@@ -693,9 +759,12 @@
     <hyperlink ref="C7" r:id="rId5" display="https://leetcode.com/problems/kth-smallest-element-in-a-bst/" xr:uid="{BC985D1B-C1C8-46C7-A4CB-631018511FEF}"/>
     <hyperlink ref="C8" r:id="rId6" display="https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/" xr:uid="{E6A98884-971B-40A3-AC5B-E52A1063EF44}"/>
     <hyperlink ref="C9" r:id="rId7" display="https://leetcode.com/problems/binary-tree-maximum-path-sum/" xr:uid="{21A06B24-7F83-4F58-A5DA-60FC2BE88869}"/>
+    <hyperlink ref="C10" r:id="rId8" display="https://leetcode.com/problems/serialize-and-deserialize-binary-tree/" xr:uid="{7058714C-DE9A-4E17-9739-F4A77B1D673F}"/>
+    <hyperlink ref="C11" r:id="rId9" display="https://leetcode.com/problems/kth-largest-element-in-a-stream/" xr:uid="{3384FF2C-C65C-4B2E-95A5-1466B2A8DDB3}"/>
+    <hyperlink ref="C12" r:id="rId10" display="https://leetcode.com/problems/last-stone-weight/" xr:uid="{331F91E0-D305-48AD-8044-48E9A28443F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 621. Task Scheduler - Dict, MaxHeap and DQ Approach
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B5AA428-D433-4950-AF22-A6366D3077A7}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16FDEB31-5B52-4A3A-908D-1B3101D75B52}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -176,6 +176,26 @@
   </si>
   <si>
     <t>Just use a heap. Re add elements to the heap again after using them (if needed). Be careful with the negatives since python max heap needs you to flip the signs</t>
+  </si>
+  <si>
+    <t>973. K Closest Points to Origin</t>
+  </si>
+  <si>
+    <t>Quick - Use a heap to track top k elements (remove any elements after k for optmization). Store elements as negative since we need to find top k.
+Optimized - In Place Quick Select (Hoare's) (REVISE IT IF YOU DON’T REMEMBER CAUSE ITS TOO LONG TO DESCRIBE HERE, CHECK GITHUB REPO)</t>
+  </si>
+  <si>
+    <t>215. Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>We first count the number of occurences of each letter with a dict (using inbuilt python func)
+Then we take only the count of values and heapify it, because we need to wait n time before doing the same task again so we start by the max occuring task so that we can fit as many small tasks in between as we need
+Then we go through the top task, decrement it to mark completion, and add it to a queue as [count, time we can do it again] at the end of the queue
+If the current time is 1 and n is 3 and we're doing task "A" which has a count of 5, we'll reduce it to 4 and increase current time to 2, and the next time we can do it again is 2 + 3 = 5, so we'll add (4, 5) to the queue
+Because of this, at each step, we'll also check if there is any task that shoud re enter the heap and pop the top of queue if true</t>
+  </si>
+  <si>
+    <t>621. Task Scheduler</t>
   </si>
 </sst>
 </file>
@@ -569,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,6 +770,48 @@
         <v>34</v>
       </c>
     </row>
+    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EF84472B-74D8-4E9E-82AC-B98F09246ED6}"/>
@@ -762,9 +824,12 @@
     <hyperlink ref="C10" r:id="rId8" display="https://leetcode.com/problems/serialize-and-deserialize-binary-tree/" xr:uid="{7058714C-DE9A-4E17-9739-F4A77B1D673F}"/>
     <hyperlink ref="C11" r:id="rId9" display="https://leetcode.com/problems/kth-largest-element-in-a-stream/" xr:uid="{3384FF2C-C65C-4B2E-95A5-1466B2A8DDB3}"/>
     <hyperlink ref="C12" r:id="rId10" display="https://leetcode.com/problems/last-stone-weight/" xr:uid="{331F91E0-D305-48AD-8044-48E9A28443F2}"/>
+    <hyperlink ref="C13" r:id="rId11" display="https://leetcode.com/problems/k-closest-points-to-origin/" xr:uid="{3D3DBF1E-36DB-412D-8476-3A3230E3EBCD}"/>
+    <hyperlink ref="C14" r:id="rId12" display="https://leetcode.com/problems/kth-largest-element-in-an-array/" xr:uid="{081CAB54-FD4F-42DA-A871-9C18F78B5A87}"/>
+    <hyperlink ref="C15" r:id="rId13" display="https://leetcode.com/problems/task-scheduler/" xr:uid="{CBFDE48C-2DAD-45DC-B364-6189E6441D85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 355. Design Twitter - Linked Lists and Heaps
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16FDEB31-5B52-4A3A-908D-1B3101D75B52}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CBE48AF-51F7-49BB-A054-5ADB6C947B49}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -196,6 +196,13 @@
   </si>
   <si>
     <t>621. Task Scheduler</t>
+  </si>
+  <si>
+    <t>Heap/PQ
+Linked Lists</t>
+  </si>
+  <si>
+    <t>355. Design Twitter</t>
   </si>
 </sst>
 </file>
@@ -281,7 +288,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -302,6 +309,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -589,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -810,6 +818,17 @@
       </c>
       <c r="D15" s="4" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -827,9 +846,10 @@
     <hyperlink ref="C13" r:id="rId11" display="https://leetcode.com/problems/k-closest-points-to-origin/" xr:uid="{3D3DBF1E-36DB-412D-8476-3A3230E3EBCD}"/>
     <hyperlink ref="C14" r:id="rId12" display="https://leetcode.com/problems/kth-largest-element-in-an-array/" xr:uid="{081CAB54-FD4F-42DA-A871-9C18F78B5A87}"/>
     <hyperlink ref="C15" r:id="rId13" display="https://leetcode.com/problems/task-scheduler/" xr:uid="{CBFDE48C-2DAD-45DC-B364-6189E6441D85}"/>
+    <hyperlink ref="C16" r:id="rId14" display="https://leetcode.com/problems/design-twitter/" xr:uid="{05673154-11C3-475F-973F-1579F327D709}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 295. Find Median from Data Stream - Naive Append & Sort Approach
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CBE48AF-51F7-49BB-A054-5ADB6C947B49}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6591E592-8D17-45FB-8AEE-8806A48E4731}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -203,6 +203,13 @@
   </si>
   <si>
     <t>355. Design Twitter</t>
+  </si>
+  <si>
+    <t>1) Twitter class stores a global variable time and users as a dict of User: { userId, tweets: Linked List of { time, tweetId, next }, followers, following } and we store each tweets with latest tweet at the front
+2) Calculate top 10 tweets by putting the heads of users and following's tweets into a max heap as (-user.tweets.time, user.tweets ) and just pop and reinsert to get the first 10. This way we basically check among all the linked lists simultaneously</t>
+  </si>
+  <si>
+    <t>Medium (!!!)</t>
   </si>
 </sst>
 </file>
@@ -288,7 +295,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -309,7 +316,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -328,10 +334,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -600,7 +602,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,24 +813,27 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solve Leetcode - 295. Find Median from Data Stream - 2 Heaps
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6591E592-8D17-45FB-8AEE-8806A48E4731}"/>
+  <xr:revisionPtr revIDLastSave="217" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CDDFAD8-527F-4B5E-B97C-3CE15A1FA058}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -157,9 +157,6 @@
     <t>297. Serialize and Deserialize Binary Tree</t>
   </si>
   <si>
-    <t>First serialize into an array using preorder traversal and then return it as string with ",".join(serialized). Next split the serialized over "," and iterate over values (maybe store the vals into an iterator with vals = iter(data) and rebuild the same way you serialized using preorder</t>
-  </si>
-  <si>
     <t>Heap/PQ</t>
   </si>
   <si>
@@ -211,12 +208,27 @@
   <si>
     <t>Medium (!!!)</t>
   </si>
+  <si>
+    <t>295. Find Median from Data Stream</t>
+  </si>
+  <si>
+    <t>First serialize into an array using preorder traversal and then return it as string with ",".join(serialized). Next split the serialized over "," and iterate over values (maybe store the vals into an iterator with vals = iter(data) and rebuild the same way you serialized using preorder.</t>
+  </si>
+  <si>
+    <t>We are essentially gonna divide the list into two sorted halves in non decreasing order with two heaps - 
+1) Left Heap will be a max heap because we need to check the rightmost element for mantaining the order or calculating median
+2) Right Heap will be a min heap because we need to check its leftmost element for aforementioned reasons
+With leftHeap[0] being &lt;= rightHeap[0], and the heaps will be approximately the same size. And we'll balance the heaps whenever we add an element.
+First check if the heaps mantain the leftHeap[-1] being &lt;= rightHeap[0] order, if not the pop fromleft and push to right in a while loop.
+Then, If the size of heaps differs by more than one element then move the top from min/max heap to the other.
+Lastly, for calculating median, if lenghts of heaps is not equal then there are odd number of elements so return that from left or right heap, otherwise there are even elements so return (leftHeap[0] + rightHeap[0]) / 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,8 +273,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +298,11 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -289,13 +313,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -316,8 +341,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -599,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,7 +657,7 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -644,7 +671,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -658,7 +685,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -672,7 +699,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -686,7 +713,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -700,7 +727,7 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -714,7 +741,7 @@
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -728,7 +755,7 @@
       <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -738,102 +765,116 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
       <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
+        <v>28</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>42</v>
+      <c r="D17" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -852,9 +893,10 @@
     <hyperlink ref="C14" r:id="rId12" display="https://leetcode.com/problems/kth-largest-element-in-an-array/" xr:uid="{081CAB54-FD4F-42DA-A871-9C18F78B5A87}"/>
     <hyperlink ref="C15" r:id="rId13" display="https://leetcode.com/problems/task-scheduler/" xr:uid="{CBFDE48C-2DAD-45DC-B364-6189E6441D85}"/>
     <hyperlink ref="C16" r:id="rId14" display="https://leetcode.com/problems/design-twitter/" xr:uid="{05673154-11C3-475F-973F-1579F327D709}"/>
+    <hyperlink ref="C17" r:id="rId15" display="https://leetcode.com/problems/find-median-from-data-stream/" xr:uid="{834858F8-92D5-4F3C-BB73-940AE43D483A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 39. Combination Sum - Backtracking
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CDDFAD8-527F-4B5E-B97C-3CE15A1FA058}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F67DBFE1-BE94-44CB-8560-AF039947D8DB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -215,13 +215,27 @@
     <t>First serialize into an array using preorder traversal and then return it as string with ",".join(serialized). Next split the serialized over "," and iterate over values (maybe store the vals into an iterator with vals = iter(data) and rebuild the same way you serialized using preorder.</t>
   </si>
   <si>
-    <t>We are essentially gonna divide the list into two sorted halves in non decreasing order with two heaps - 
+    <t>(Small and elegant version is this, more comprehensive verssion is below)
+Use a maxHeap for the smaller half of numbers and a minHeap for the larger half.
+Always insert into maxHeap first (as negative), then move its largest element to minHeap so that all elements in maxHeap &lt;= all elements in minHeap.
+If minHeap becomes larger, move its smallest back to maxHeap to maintain size balance (maxHeap can have equal size or one extra element).
+Median is either the top of maxHeap (odd total size) or the average of both tops (even size).
+We are essentially gonna divide the list into two sorted halves in non decreasing order with two heaps - 
 1) Left Heap will be a max heap because we need to check the rightmost element for mantaining the order or calculating median
 2) Right Heap will be a min heap because we need to check its leftmost element for aforementioned reasons
 With leftHeap[0] being &lt;= rightHeap[0], and the heaps will be approximately the same size. And we'll balance the heaps whenever we add an element.
 First check if the heaps mantain the leftHeap[-1] being &lt;= rightHeap[0] order, if not the pop fromleft and push to right in a while loop.
 Then, If the size of heaps differs by more than one element then move the top from min/max heap to the other.
 Lastly, for calculating median, if lenghts of heaps is not equal then there are odd number of elements so return that from left or right heap, otherwise there are even elements so return (leftHeap[0] + rightHeap[0]) / 2</t>
+  </si>
+  <si>
+    <t>Backtracking</t>
+  </si>
+  <si>
+    <t>78. Subsets</t>
+  </si>
+  <si>
+    <t>For each element, we can either add it to res or not add it. Run a recursive backtrack function with a curr variable for list and i for tracking nums indices. And do curr.append(nums[i]) then backtrack and then curr.pop() then backtrack. Base case will be i goes out of bounds, then we need to add (a copy of) curr to res. Return res in the end</t>
   </si>
 </sst>
 </file>
@@ -361,6 +375,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -626,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,7 +881,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -875,6 +893,20 @@
       </c>
       <c r="D17" s="4" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -894,9 +926,10 @@
     <hyperlink ref="C15" r:id="rId13" display="https://leetcode.com/problems/task-scheduler/" xr:uid="{CBFDE48C-2DAD-45DC-B364-6189E6441D85}"/>
     <hyperlink ref="C16" r:id="rId14" display="https://leetcode.com/problems/design-twitter/" xr:uid="{05673154-11C3-475F-973F-1579F327D709}"/>
     <hyperlink ref="C17" r:id="rId15" display="https://leetcode.com/problems/find-median-from-data-stream/" xr:uid="{834858F8-92D5-4F3C-BB73-940AE43D483A}"/>
+    <hyperlink ref="C18" r:id="rId16" display="https://leetcode.com/problems/subsets/" xr:uid="{B506B266-0541-48BA-80A1-3BF94E526EA1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 40. Combination Sum II - Backtracking (with and without for loop)
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F67DBFE1-BE94-44CB-8560-AF039947D8DB}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FACA65A2-953C-464E-8780-7A4E8F356662}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -236,6 +236,25 @@
   </si>
   <si>
     <t>For each element, we can either add it to res or not add it. Run a recursive backtrack function with a curr variable for list and i for tracking nums indices. And do curr.append(nums[i]) then backtrack and then curr.pop() then backtrack. Base case will be i goes out of bounds, then we need to add (a copy of) curr to res. Return res in the end</t>
+  </si>
+  <si>
+    <t>39. Combination Sum</t>
+  </si>
+  <si>
+    <t>For each element, we have a choice whether to pick and and keep picking it again and again, or not pick it. So we do a greedy search with a recursive function where we track running sum in rsum and current elements picked in curr
+For each element we either add it to curr and rsum and backtrack, or we dont add it and move over to next element and backtrack
+If rsum == target then add it to res, or if rsum crosses target or i goes out of bounds, we just return and return the final answer in the end</t>
+  </si>
+  <si>
+    <t>Medium (!)</t>
+  </si>
+  <si>
+    <t>We first need to sort the array (this note assumes its non decreasing) and for each candidate starting at index i, either pick it (add to curr, rsum -= candidate) and recurse, or move to the next candidate in the loop.
+Skip duplicates at the same depth: if j &gt; i and candidates[j] == candidates[j-1]: continue.
+When rsum == 0, append a copy of curr to res. Stop recursion if rsum &lt; 0 or i goes out of bounds.</t>
+  </si>
+  <si>
+    <t>40. Combination Sum II</t>
   </si>
 </sst>
 </file>
@@ -375,10 +394,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -644,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,13 +915,41 @@
         <v>46</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -927,9 +970,11 @@
     <hyperlink ref="C16" r:id="rId14" display="https://leetcode.com/problems/design-twitter/" xr:uid="{05673154-11C3-475F-973F-1579F327D709}"/>
     <hyperlink ref="C17" r:id="rId15" display="https://leetcode.com/problems/find-median-from-data-stream/" xr:uid="{834858F8-92D5-4F3C-BB73-940AE43D483A}"/>
     <hyperlink ref="C18" r:id="rId16" display="https://leetcode.com/problems/subsets/" xr:uid="{B506B266-0541-48BA-80A1-3BF94E526EA1}"/>
+    <hyperlink ref="C19" r:id="rId17" display="https://leetcode.com/problems/combination-sum/" xr:uid="{339DFEA2-EC97-463B-91E3-40FCC5215C19}"/>
+    <hyperlink ref="C20" r:id="rId18" display="https://leetcode.com/problems/combination-sum-ii/" xr:uid="{010D4CB3-590E-4139-97F7-B813500511B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 90. Subsets II - Subsets
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="248" documentId="11_F25DC773A252ABDACC104834211F6EBC5ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FACA65A2-953C-464E-8780-7A4E8F356662}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -255,6 +255,80 @@
   </si>
   <si>
     <t>40. Combination Sum II</t>
+  </si>
+  <si>
+    <t>46. Permutations</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Break down (Recursive ans) or Build up (Iterative ans) to the answer. Permutations for [1] is just [[1]] right, for [1,2] its [[1,2],[2,1]], which is just permutation of [1] but with 2 inserted at all possible indices, and same for [1,2,3] and so on.
+(Also do not modify any element of res directly, make a copy first)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recursive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> have base case be nums == 0: return [[]]. Then recusively get permutations for nums[1:] and store it in perms, after that just insert nums[0] at all possible positions, store it in a res variable and return res.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Iterative - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>start with res = [[]]. Outermost loop loops over all nums, then go over each list in res, and then go over each index and insert the selected num at all possible positions. Append to a temp array since we cannot modify res while looping over it and then replace res with temp and return res in the end.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -659,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,6 +1024,20 @@
       </c>
       <c r="D20" s="4" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -972,9 +1060,10 @@
     <hyperlink ref="C18" r:id="rId16" display="https://leetcode.com/problems/subsets/" xr:uid="{B506B266-0541-48BA-80A1-3BF94E526EA1}"/>
     <hyperlink ref="C19" r:id="rId17" display="https://leetcode.com/problems/combination-sum/" xr:uid="{339DFEA2-EC97-463B-91E3-40FCC5215C19}"/>
     <hyperlink ref="C20" r:id="rId18" display="https://leetcode.com/problems/combination-sum-ii/" xr:uid="{010D4CB3-590E-4139-97F7-B813500511B5}"/>
+    <hyperlink ref="C21" r:id="rId19" display="https://leetcode.com/problems/permutations/" xr:uid="{8107E641-A58A-4879-8D24-89021B858F52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 79. Word Search - Backtracking
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{225A8BAB-DCF9-46F7-B14C-35D068341E88}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -329,6 +329,13 @@
       </rPr>
       <t>start with res = [[]]. Outermost loop loops over all nums, then go over each list in res, and then go over each index and insert the selected num at all possible positions. Append to a temp array since we cannot modify res while looping over it and then replace res with temp and return res in the end.</t>
     </r>
+  </si>
+  <si>
+    <t>90. Subsets II</t>
+  </si>
+  <si>
+    <t>Same as LC 78. Subsets but we sort the input and skip duplicates at the same level (by checking j &gt; i and nums[j - 1] == nums[j]): continue
+Sorting is needed since some input could be like [4, 4, 1, 4] and then nums[j - 1] == nums[j] logic will break</t>
   </si>
 </sst>
 </file>
@@ -733,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,6 +1045,20 @@
       </c>
       <c r="D21" s="4" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1061,9 +1082,10 @@
     <hyperlink ref="C19" r:id="rId17" display="https://leetcode.com/problems/combination-sum/" xr:uid="{339DFEA2-EC97-463B-91E3-40FCC5215C19}"/>
     <hyperlink ref="C20" r:id="rId18" display="https://leetcode.com/problems/combination-sum-ii/" xr:uid="{010D4CB3-590E-4139-97F7-B813500511B5}"/>
     <hyperlink ref="C21" r:id="rId19" display="https://leetcode.com/problems/permutations/" xr:uid="{8107E641-A58A-4879-8D24-89021B858F52}"/>
+    <hyperlink ref="C22" r:id="rId20" display="https://leetcode.com/problems/subsets-ii/" xr:uid="{BB3DCCD4-C3F0-4739-9456-F789A1338E36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 131. Palindrome Partitioning - Backtracking
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{225A8BAB-DCF9-46F7-B14C-35D068341E88}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24F288DB-5125-4328-AB96-25A322862D72}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -336,6 +336,38 @@
   <si>
     <t>Same as LC 78. Subsets but we sort the input and skip duplicates at the same level (by checking j &gt; i and nums[j - 1] == nums[j]): continue
 Sorting is needed since some input could be like [4, 4, 1, 4] and then nums[j - 1] == nums[j] logic will break</t>
+  </si>
+  <si>
+    <t>79. Word Search</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We basically need to run a dfs with backtracking. First find the starting word in the matrix and then run dfs(rowIdx, colIdx, 0) search from that element and return True if dfs returns true as its final return value, otherwise return False at the end.
+Base case will be return True if check and match upto the last letter of word, or  False if `the row or col idx is out of bounds, or the word does not match, or if its already visited.
+Add the current element to a set or mark it in the matrix with "#" to signify we have visited it, then check the top, bottom, left and right element for the next word match recursively, then de mark it and return the result of the checks we ran.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Optimizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - If word length &gt; matrix size then return False immediately. Count the frequency of all letters in matrix, if frequency of starting letter is more than ending letter then flip it (since then we'd have to run lesser dfs searches)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -475,6 +507,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -740,7 +776,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
@@ -1059,6 +1095,20 @@
       </c>
       <c r="D22" s="4" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1083,9 +1133,10 @@
     <hyperlink ref="C20" r:id="rId18" display="https://leetcode.com/problems/combination-sum-ii/" xr:uid="{010D4CB3-590E-4139-97F7-B813500511B5}"/>
     <hyperlink ref="C21" r:id="rId19" display="https://leetcode.com/problems/permutations/" xr:uid="{8107E641-A58A-4879-8D24-89021B858F52}"/>
     <hyperlink ref="C22" r:id="rId20" display="https://leetcode.com/problems/subsets-ii/" xr:uid="{BB3DCCD4-C3F0-4739-9456-F789A1338E36}"/>
+    <hyperlink ref="C23" r:id="rId21" display="https://leetcode.com/problems/word-search/" xr:uid="{FED0AF81-7B9A-477C-B9DE-B27A86798AE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add explanation to Leetcode - 131. Palindrome Partitioning - Backtracking
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24F288DB-5125-4328-AB96-25A322862D72}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EE8965D-5F43-4A1D-BD7C-D301BCC19280}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Neetcode 150" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -368,6 +368,15 @@
       </rPr>
       <t xml:space="preserve"> - If word length &gt; matrix size then return False immediately. Count the frequency of all letters in matrix, if frequency of starting letter is more than ending letter then flip it (since then we'd have to run lesser dfs searches)</t>
     </r>
+  </si>
+  <si>
+    <t>131. Palindrome Partitioning</t>
+  </si>
+  <si>
+    <t>The basic idea is - Whats the biggest palindrome partition we can get from i to j
+We run a for loop j in range(i, len(s)), in that we check for partition slice from i to j, if its valid append that slice to curr and run dfs(j + 1) to solve for the rest of the array, after that pop the slice we appended, so that we can look at a bigger slice in the next iteration of the loop.
+In the next iteration j will move and our window will get bigger, if the slice is a partiton append it to curr again and look at the  rest of the array, otherwise we dont need to look at this branch any longer.
+BASECASE: We need to find the final array after finding out all combos of the partitions, so add to res only when i &gt;= n</t>
   </si>
 </sst>
 </file>
@@ -776,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1109,6 +1118,20 @@
       </c>
       <c r="D23" s="4" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1134,9 +1157,10 @@
     <hyperlink ref="C21" r:id="rId19" display="https://leetcode.com/problems/permutations/" xr:uid="{8107E641-A58A-4879-8D24-89021B858F52}"/>
     <hyperlink ref="C22" r:id="rId20" display="https://leetcode.com/problems/subsets-ii/" xr:uid="{BB3DCCD4-C3F0-4739-9456-F789A1338E36}"/>
     <hyperlink ref="C23" r:id="rId21" display="https://leetcode.com/problems/word-search/" xr:uid="{FED0AF81-7B9A-477C-B9DE-B27A86798AE6}"/>
+    <hyperlink ref="C24" r:id="rId22" display="https://leetcode.com/problems/palindrome-partitioning/" xr:uid="{1004F407-D991-4482-844C-624178374F24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 17. Letter Combinations of a Phone Number - Backtracking
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EE8965D-5F43-4A1D-BD7C-D301BCC19280}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82D80E23-21D7-4A21-8AFB-10438CECAE8D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -377,6 +377,13 @@
 We run a for loop j in range(i, len(s)), in that we check for partition slice from i to j, if its valid append that slice to curr and run dfs(j + 1) to solve for the rest of the array, after that pop the slice we appended, so that we can look at a bigger slice in the next iteration of the loop.
 In the next iteration j will move and our window will get bigger, if the slice is a partiton append it to curr again and look at the  rest of the array, otherwise we dont need to look at this branch any longer.
 BASECASE: We need to find the final array after finding out all combos of the partitions, so add to res only when i &gt;= n</t>
+  </si>
+  <si>
+    <t>17. Letter Combinations of a Phone Number</t>
+  </si>
+  <si>
+    <t>Store the letters in an array like ["abc", "def", ...] and convert digits (eg. "23" to 01) so that we can correspond it with the array easier
+Run a recursive dfs, at each level, pick each digit in a loop and recurse to next level, until we reach base case i &gt;= n, then append to res with "".join(curr) and then pop out the digit after using it</t>
   </si>
 </sst>
 </file>
@@ -785,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,6 +1139,20 @@
       </c>
       <c r="D24" s="4" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1158,9 +1179,10 @@
     <hyperlink ref="C22" r:id="rId20" display="https://leetcode.com/problems/subsets-ii/" xr:uid="{BB3DCCD4-C3F0-4739-9456-F789A1338E36}"/>
     <hyperlink ref="C23" r:id="rId21" display="https://leetcode.com/problems/word-search/" xr:uid="{FED0AF81-7B9A-477C-B9DE-B27A86798AE6}"/>
     <hyperlink ref="C24" r:id="rId22" display="https://leetcode.com/problems/palindrome-partitioning/" xr:uid="{1004F407-D991-4482-844C-624178374F24}"/>
+    <hyperlink ref="C25" r:id="rId23" display="https://leetcode.com/problems/letter-combinations-of-a-phone-number/" xr:uid="{3FBAA95B-9DFD-40D6-B70D-F8C257E0F774}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 51. N-Queens - Optimal Time solution
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82D80E23-21D7-4A21-8AFB-10438CECAE8D}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0A062A8-711B-4CB9-BF19-537757E60F98}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Neetcode 150" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -384,6 +384,74 @@
   <si>
     <t>Store the letters in an array like ["abc", "def", ...] and convert digits (eg. "23" to 01) so that we can correspond it with the array easier
 Run a recursive dfs, at each level, pick each digit in a loop and recurse to next level, until we reach base case i &gt;= n, then append to res with "".join(curr) and then pop out the digit after using it</t>
+  </si>
+  <si>
+    <t>51. N-Queens</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OPTIMAL SPACE - O(N) CONFLICT CHECK)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Store only queen column positions in queens=[-1]*n array instead of full n×n board to save space and reconstruct to full board when adding to res. Handle collisions:
+Row: Each queen gets own row (implicit in backtracking)
+Col: Loop through previous rows, check if col==usedCol
+Diagonal: Use slope property abs(r2-r1)==abs(c2-c1) to check if current and any previous queen share a diagonal
+(Mathematically, for a line to be considered a slope, at each point, it would be increasing/decreasing along the x/y axis by an EQUAL DEGREE, if thats true, then its 100% a slope. diagonal lines increase/decrease by EQUAL amounts in both axes, so equal absolute differences means same diagonal))
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OPTIMAL TIME - O(1) CONFLICT CHECK)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Store queen positions in queens=[-1]*n AND track conflicts in three sets and add to sets when placing, remove when backtracking. -
+cols set: blocked columns
+pos set: positive diagonals (row+col) - cells on same / diagonal have same sum because (row-1)+(col+1)=row+col stays constant
+neg set: negative diagonals (row-col) - cells on same \ diagonal have same difference because (row+1)-(col+1)=row-col stays constant
+Before placing queen at [row][col], check: col not in cols AND (row+col) not in pos AND (row-col) not in neg</t>
+    </r>
+  </si>
+  <si>
+    <t>Tries</t>
+  </si>
+  <si>
+    <t>208. Implement Trie (Prefix Tree)</t>
+  </si>
+  <si>
+    <t>Trie can be defined as a hashmap of hasmap. It is optimized for string based data reTRIEval, ip routing, dictionaries etc.
+Just create a TrieNode class that has a nodes = dict() for next set of tries and end property to denote that a word ends here. Traverse by checking for each letter in word and go level by level, thats all the info you need.</t>
   </si>
 </sst>
 </file>
@@ -792,17 +860,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14.21875" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="114" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="115.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="115.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1153,6 +1222,34 @@
       </c>
       <c r="D25" s="4" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1180,9 +1277,10 @@
     <hyperlink ref="C23" r:id="rId21" display="https://leetcode.com/problems/word-search/" xr:uid="{FED0AF81-7B9A-477C-B9DE-B27A86798AE6}"/>
     <hyperlink ref="C24" r:id="rId22" display="https://leetcode.com/problems/palindrome-partitioning/" xr:uid="{1004F407-D991-4482-844C-624178374F24}"/>
     <hyperlink ref="C25" r:id="rId23" display="https://leetcode.com/problems/letter-combinations-of-a-phone-number/" xr:uid="{3FBAA95B-9DFD-40D6-B70D-F8C257E0F774}"/>
+    <hyperlink ref="C27" r:id="rId24" display="https://leetcode.com/problems/implement-trie-prefix-tree/" xr:uid="{CB4E4F7A-E67A-473D-A51C-23D207D85118}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 212. Word Search II
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{83538C8C-D055-47D4-91D2-8AEEED051D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0A062A8-711B-4CB9-BF19-537757E60F98}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03F23B5-14D5-45B3-BEE4-50F12280368E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -452,6 +452,16 @@
   <si>
     <t>Trie can be defined as a hashmap of hasmap. It is optimized for string based data reTRIEval, ip routing, dictionaries etc.
 Just create a TrieNode class that has a nodes = dict() for next set of tries and end property to denote that a word ends here. Traverse by checking for each letter in word and go level by level, thats all the info you need.</t>
+  </si>
+  <si>
+    <t>211. Design Add and Search Words Data Structure</t>
+  </si>
+  <si>
+    <t>Just split the word by chars and put it in the Trie one by one, create a TrieNode( nodes: {}, end: boolean ) for each missing node
+search function should take the word, starting idx (default 0) and the TrieNode to start the search from (default None, set to the root of Trie
+if its None (can't set default value with self in default args in python)) and search normally with curr for any char
+If we see a "." then switch the approach and run search again for each child in current TrieNode's children from the i + 1 char
+Do the same for any subsequent "." and immediately return True if a recursive search returns true. Else return false</t>
   </si>
 </sst>
 </file>
@@ -591,10 +601,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -860,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,6 +1256,20 @@
       </c>
       <c r="D27" s="4" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1278,9 +1298,10 @@
     <hyperlink ref="C24" r:id="rId22" display="https://leetcode.com/problems/palindrome-partitioning/" xr:uid="{1004F407-D991-4482-844C-624178374F24}"/>
     <hyperlink ref="C25" r:id="rId23" display="https://leetcode.com/problems/letter-combinations-of-a-phone-number/" xr:uid="{3FBAA95B-9DFD-40D6-B70D-F8C257E0F774}"/>
     <hyperlink ref="C27" r:id="rId24" display="https://leetcode.com/problems/implement-trie-prefix-tree/" xr:uid="{CB4E4F7A-E67A-473D-A51C-23D207D85118}"/>
+    <hyperlink ref="C28" r:id="rId25" display="https://leetcode.com/problems/design-add-and-search-words-data-structure/" xr:uid="{E928019A-72A2-4A36-9E55-D2897C0322B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 200. Number of Islands - DFS
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03F23B5-14D5-45B3-BEE4-50F12280368E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BE5679-F523-4C54-9D17-20424CD142DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -462,6 +462,21 @@
 if its None (can't set default value with self in default args in python)) and search normally with curr for any char
 If we see a "." then switch the approach and run search again for each child in current TrieNode's children from the i + 1 char
 Do the same for any subsequent "." and immediately return True if a recursive search returns true. Else return false</t>
+  </si>
+  <si>
+    <t>212. Word Search II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The basic idea is we first create a trie for each node and then we iterater over the matrix and check for starting positions of a word in the trie
+If we find it then we run a dfs in all 4 directions (mark visited as #) and see if we can check off words along the way. (check off "OAT" while
+looking for "OATH") and add it to res if any word ends at current letter (by checking TreeNode's word property which should contain the whole word)
+For optimization we clear the visited words from the Trie and delete the tree branch if all curr.nodes have been visited.
+1. First put all the words in a Trie (Also use curr.word instead of curr.end, so that we can quickly get the word we need to add to res)
+2. Then, iterate over the matrix and run dfs for each letter and pass the root node of the trie
+3. The base case for dfs will be if row/col is out of bounds or the current letter is not in curr.nodes.
+4. Then save curr as parent (We need this for pruning) AND THEN move curr over to be its next value. We also mark board[row][col] as "#" (after saving the original value) so that we dont add the same letter and we can change it back
+5. We check if a word ends at this node by checking curr.word (which should have the full word that ends there) and add it to res and set it to None.
+6. Then we run dfs for all 4 directions and for optimization, delete curr if it has no children, it's a dead-end path. We delete it from its parent node to prevent future DFS calls from exploring this useless branch. </t>
   </si>
 </sst>
 </file>
@@ -866,9 +881,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1270,6 +1285,20 @@
       </c>
       <c r="D28" s="4" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="217.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1299,9 +1328,10 @@
     <hyperlink ref="C25" r:id="rId23" display="https://leetcode.com/problems/letter-combinations-of-a-phone-number/" xr:uid="{3FBAA95B-9DFD-40D6-B70D-F8C257E0F774}"/>
     <hyperlink ref="C27" r:id="rId24" display="https://leetcode.com/problems/implement-trie-prefix-tree/" xr:uid="{CB4E4F7A-E67A-473D-A51C-23D207D85118}"/>
     <hyperlink ref="C28" r:id="rId25" display="https://leetcode.com/problems/design-add-and-search-words-data-structure/" xr:uid="{E928019A-72A2-4A36-9E55-D2897C0322B4}"/>
+    <hyperlink ref="C29" r:id="rId26" display="https://leetcode.com/problems/word-search-ii/" xr:uid="{2AE3B4BB-82A6-4559-85C0-0F858438646A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 200. Number of Islands - BFS
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BE5679-F523-4C54-9D17-20424CD142DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{35BE5679-F523-4C54-9D17-20424CD142DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B124106C-798E-4335-8A63-DBB25F13B5E3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="76">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -477,6 +477,15 @@
 4. Then save curr as parent (We need this for pruning) AND THEN move curr over to be its next value. We also mark board[row][col] as "#" (after saving the original value) so that we dont add the same letter and we can change it back
 5. We check if a word ends at this node by checking curr.word (which should have the full word that ends there) and add it to res and set it to None.
 6. Then we run dfs for all 4 directions and for optimization, delete curr if it has no children, it's a dead-end path. We delete it from its parent node to prevent future DFS calls from exploring this useless branch. </t>
+  </si>
+  <si>
+    <t>Graphs</t>
+  </si>
+  <si>
+    <t>200. Number of Islands</t>
+  </si>
+  <si>
+    <t>Whenever we encounter an island ("1"), run a dfs with all 4 directions to mark the entire island "#" for visited and increment res. Then go find the next island</t>
   </si>
 </sst>
 </file>
@@ -881,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1299,6 +1308,20 @@
       </c>
       <c r="D29" s="4" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1329,9 +1352,10 @@
     <hyperlink ref="C27" r:id="rId24" display="https://leetcode.com/problems/implement-trie-prefix-tree/" xr:uid="{CB4E4F7A-E67A-473D-A51C-23D207D85118}"/>
     <hyperlink ref="C28" r:id="rId25" display="https://leetcode.com/problems/design-add-and-search-words-data-structure/" xr:uid="{E928019A-72A2-4A36-9E55-D2897C0322B4}"/>
     <hyperlink ref="C29" r:id="rId26" display="https://leetcode.com/problems/word-search-ii/" xr:uid="{2AE3B4BB-82A6-4559-85C0-0F858438646A}"/>
+    <hyperlink ref="C30" r:id="rId27" display="https://leetcode.com/problems/number-of-islands/" xr:uid="{64D08A58-4025-4F89-A8A2-73BCF2F52AC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 133. Clone Graph - DFS
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{35BE5679-F523-4C54-9D17-20424CD142DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B124106C-798E-4335-8A63-DBB25F13B5E3}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{35BE5679-F523-4C54-9D17-20424CD142DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4957B6B-1195-4FCB-B3E4-9D46FE665C93}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -486,6 +486,12 @@
   </si>
   <si>
     <t>Whenever we encounter an island ("1"), run a dfs with all 4 directions to mark the entire island "#" for visited and increment res. Then go find the next island</t>
+  </si>
+  <si>
+    <t>695. Max Area of Island</t>
+  </si>
+  <si>
+    <t>Whenever we encounter an island ("1"), run a dfs with all 4 directions to mark the entire island "#" for visited and track cur_max and max_max. Then go find the next island</t>
   </si>
 </sst>
 </file>
@@ -625,6 +631,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -890,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,6 +1332,20 @@
       </c>
       <c r="D30" s="4" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1353,9 +1377,10 @@
     <hyperlink ref="C28" r:id="rId25" display="https://leetcode.com/problems/design-add-and-search-words-data-structure/" xr:uid="{E928019A-72A2-4A36-9E55-D2897C0322B4}"/>
     <hyperlink ref="C29" r:id="rId26" display="https://leetcode.com/problems/word-search-ii/" xr:uid="{2AE3B4BB-82A6-4559-85C0-0F858438646A}"/>
     <hyperlink ref="C30" r:id="rId27" display="https://leetcode.com/problems/number-of-islands/" xr:uid="{64D08A58-4025-4F89-A8A2-73BCF2F52AC0}"/>
+    <hyperlink ref="C31" r:id="rId28" display="https://leetcode.com/problems/max-area-of-island/" xr:uid="{9F1FA12C-B15D-4CF8-A7D8-EE6F3DB615C1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 286. Walls and Gates - Multi Source BFS and DFS
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{35BE5679-F523-4C54-9D17-20424CD142DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4957B6B-1195-4FCB-B3E4-9D46FE665C93}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDED84F3-0051-4AAC-8580-B1C1B687D42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -492,6 +492,20 @@
   </si>
   <si>
     <t>Whenever we encounter an island ("1"), run a dfs with all 4 directions to mark the entire island "#" for visited and track cur_max and max_max. Then go find the next island</t>
+  </si>
+  <si>
+    <t>133. Clone Graph</t>
+  </si>
+  <si>
+    <t>We need to create a copy for each node in the graph, and we'll track those copies with a hashap
+Then, run a dfs with base case node is already in hashmap then just return it from the hashmap otherwise create the node, add it to hashmap and run dfs again recursively for each neighbour and append what it returns to copy's neighbors, and return the copy after going through all neighbors</t>
+  </si>
+  <si>
+    <t>286. Walls and Gates</t>
+  </si>
+  <si>
+    <t>Multi Source BFS is just like bfs except we start with multiple root nodes and move deeper for all nodes consecutively.
+First find all 0's, those will be the roots for the multi source bfs, then run the usual bfs exapnding in all 4 directions, and for each direction, add it to bfs if its indices are within bounds and if its value is &lt;= current val + 1, only then overwrite its dist and add it to null to ensure that we only overwrite to make paths shorter, not longer.</t>
   </si>
 </sst>
 </file>
@@ -631,10 +645,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -900,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1346,6 +1356,34 @@
       </c>
       <c r="D31" s="4" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1378,9 +1416,11 @@
     <hyperlink ref="C29" r:id="rId26" display="https://leetcode.com/problems/word-search-ii/" xr:uid="{2AE3B4BB-82A6-4559-85C0-0F858438646A}"/>
     <hyperlink ref="C30" r:id="rId27" display="https://leetcode.com/problems/number-of-islands/" xr:uid="{64D08A58-4025-4F89-A8A2-73BCF2F52AC0}"/>
     <hyperlink ref="C31" r:id="rId28" display="https://leetcode.com/problems/max-area-of-island/" xr:uid="{9F1FA12C-B15D-4CF8-A7D8-EE6F3DB615C1}"/>
+    <hyperlink ref="C32" r:id="rId29" display="https://leetcode.com/problems/clone-graph/" xr:uid="{798CD2A6-9011-4AEF-AF71-D506F15BADE9}"/>
+    <hyperlink ref="C33" r:id="rId30" xr:uid="{10F2E698-8B08-4256-A73C-09AAACB3036A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 994. Rotting Oranges - Multi Source BFS
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDED84F3-0051-4AAC-8580-B1C1B687D42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBBFE6E-443F-4AE5-870A-8C0854D767CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -506,6 +506,12 @@
   <si>
     <t>Multi Source BFS is just like bfs except we start with multiple root nodes and move deeper for all nodes consecutively.
 First find all 0's, those will be the roots for the multi source bfs, then run the usual bfs exapnding in all 4 directions, and for each direction, add it to bfs if its indices are within bounds and if its value is &lt;= current val + 1, only then overwrite its dist and add it to null to ensure that we only overwrite to make paths shorter, not longer.</t>
+  </si>
+  <si>
+    <t>Just run a multi source bfs, and track the number of fresh fruits. while q and fruits &gt; 0, then go down level by level in bfs with for _ in range(len(q)) and increment time everytime we go down a level. In the end return -1 if there are fresh fruits left, otherwise return time</t>
+  </si>
+  <si>
+    <t>994. Rotting Oranges</t>
   </si>
 </sst>
 </file>
@@ -910,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,6 +1390,20 @@
       </c>
       <c r="D33" s="4" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1418,9 +1438,10 @@
     <hyperlink ref="C31" r:id="rId28" display="https://leetcode.com/problems/max-area-of-island/" xr:uid="{9F1FA12C-B15D-4CF8-A7D8-EE6F3DB615C1}"/>
     <hyperlink ref="C32" r:id="rId29" display="https://leetcode.com/problems/clone-graph/" xr:uid="{798CD2A6-9011-4AEF-AF71-D506F15BADE9}"/>
     <hyperlink ref="C33" r:id="rId30" xr:uid="{10F2E698-8B08-4256-A73C-09AAACB3036A}"/>
+    <hyperlink ref="C34" r:id="rId31" display="https://leetcode.com/problems/rotting-oranges/" xr:uid="{15EA9BCE-06C4-4EEB-9796-6DABB67D400E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 130. Surrounded Regions
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBBFE6E-443F-4AE5-870A-8C0854D767CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC2C32F-E44C-446C-A44E-0B3E03F1B9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="86">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -512,6 +512,13 @@
   </si>
   <si>
     <t>994. Rotting Oranges</t>
+  </si>
+  <si>
+    <t>417. Pacific Atlantic Water Flow (!)</t>
+  </si>
+  <si>
+    <t>The core idea is that, instead of going from each cell and checking all sides recursively with dfs to see if it can reach both the oceans,
+We start our search from the boundaries (top row, bot row, left col, right col), where its guarenteed its touching the ocean, from that we run the dfs. And we track each cell with its corresponding ocean set, so theres no redundant traversal, and we only proceed with the dfs if its a valid cell ie. index within bounds, prev height &lt; curr height, curr not in set</t>
   </si>
 </sst>
 </file>
@@ -916,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1404,6 +1411,20 @@
       </c>
       <c r="D34" s="4" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1439,9 +1460,10 @@
     <hyperlink ref="C32" r:id="rId29" display="https://leetcode.com/problems/clone-graph/" xr:uid="{798CD2A6-9011-4AEF-AF71-D506F15BADE9}"/>
     <hyperlink ref="C33" r:id="rId30" xr:uid="{10F2E698-8B08-4256-A73C-09AAACB3036A}"/>
     <hyperlink ref="C34" r:id="rId31" display="https://leetcode.com/problems/rotting-oranges/" xr:uid="{15EA9BCE-06C4-4EEB-9796-6DABB67D400E}"/>
+    <hyperlink ref="C35" r:id="rId32" display="https://leetcode.com/problems/pacific-atlantic-water-flow/" xr:uid="{A5087F08-C7AB-4992-B57F-A7D1AA6DD6C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 207. Course Schedule - DFS
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC2C32F-E44C-446C-A44E-0B3E03F1B9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{6BC2C32F-E44C-446C-A44E-0B3E03F1B9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7F267B6-AE9C-41E5-AE27-78927F65EC4C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Neetcode 150" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -519,6 +519,13 @@
   <si>
     <t>The core idea is that, instead of going from each cell and checking all sides recursively with dfs to see if it can reach both the oceans,
 We start our search from the boundaries (top row, bot row, left col, right col), where its guarenteed its touching the ocean, from that we run the dfs. And we track each cell with its corresponding ocean set, so theres no redundant traversal, and we only proceed with the dfs if its a valid cell ie. index within bounds, prev height &lt; curr height, curr not in set</t>
+  </si>
+  <si>
+    <t>130. Surrounded Regions</t>
+  </si>
+  <si>
+    <t>Any region of O cannot be flipped if its connected to the boundares, so we just check from the boundaries, find the starting of a region on the row and col boundaries, and then mark the entire region as "#" so we definitely know we cant flip it, then the regions of "O"'s which are left would be "islands", which we can flip
+Then just go through the array and flip those, and also turn the invalid regions we changed to "#" back to "O" and we're done.</t>
   </si>
 </sst>
 </file>
@@ -923,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1425,6 +1432,20 @@
       </c>
       <c r="D35" s="4" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1461,9 +1482,10 @@
     <hyperlink ref="C33" r:id="rId30" xr:uid="{10F2E698-8B08-4256-A73C-09AAACB3036A}"/>
     <hyperlink ref="C34" r:id="rId31" display="https://leetcode.com/problems/rotting-oranges/" xr:uid="{15EA9BCE-06C4-4EEB-9796-6DABB67D400E}"/>
     <hyperlink ref="C35" r:id="rId32" display="https://leetcode.com/problems/pacific-atlantic-water-flow/" xr:uid="{A5087F08-C7AB-4992-B57F-A7D1AA6DD6C9}"/>
+    <hyperlink ref="C36" r:id="rId33" display="https://leetcode.com/problems/surrounded-regions/" xr:uid="{2D073E62-CEDC-4D3A-9478-1237B343B174}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId33"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 261. Graph Valid Tree - BFS
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{6BC2C32F-E44C-446C-A44E-0B3E03F1B9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7F267B6-AE9C-41E5-AE27-78927F65EC4C}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{6BC2C32F-E44C-446C-A44E-0B3E03F1B9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFA78C88-DC04-4592-9325-BA395CBD987A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Neetcode 150" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -526,6 +526,30 @@
   <si>
     <t>Any region of O cannot be flipped if its connected to the boundares, so we just check from the boundaries, find the starting of a region on the row and col boundaries, and then mark the entire region as "#" so we definitely know we cant flip it, then the regions of "O"'s which are left would be "islands", which we can flip
 Then just go through the array and flip those, and also turn the invalid regions we changed to "#" back to "O" and we're done.</t>
+  </si>
+  <si>
+    <t>207. Course Schedule</t>
+  </si>
+  <si>
+    <t>210. Course Schedule II</t>
+  </si>
+  <si>
+    <t>check this article for more details - https://mohammad-imran.medium.com/understanding-topological-sorting-with-kahns-algo-8af5a588dd0e
+We see whether Topological sorting with Kahn's algorithm would have printed nodes == numCourses or not. Topological sorting in graphs is just dfs + print/action at the deepest level, bubbling up.
+Kahs's Algorithm variant is - first make an adjacency graph for all vertices and edge direction, and indegree (how many edges points to current)
+then do a multi source BFS with all indegree[i] == 0, remove all the edges that originate from this current vertex from indegree for all current's edges and add indegree[i] to the queue if its its value is 0, repeat until all inorder[i] == 0 (success) or all inorder[i] &gt; 0 (fail, because of cycle)</t>
+  </si>
+  <si>
+    <t>Exactly the same as above (Course Schedule 1 - Kahn's Algo Topo Sort) +
+An additional thing we do is append the curr node to res, and return res if canComplete == numCourses else []</t>
+  </si>
+  <si>
+    <t>261. Graph Valid Tree</t>
+  </si>
+  <si>
+    <t>Make a bi-directional adjacency matrix (WITH SETS) and add each edge and its inverse ((0, 1) and (1, 0))
+We'll do BFS so make a deque and a seen set for traversal and add 0 to both, then traverse LEVEL BY LEVEL and loop over curr nodes children and check if any of them are in seen (a cycle is found)
+Then add child to seen and remove curr from the child's neighbours set (adj[child]) (so we dont go back and do an infinite loop) return len(seen) == n to check if we have visited all nodes (unvisited/disconnected node means not a tree)</t>
   </si>
 </sst>
 </file>
@@ -665,6 +689,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -930,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1446,6 +1474,48 @@
       </c>
       <c r="D36" s="4" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1483,9 +1553,12 @@
     <hyperlink ref="C34" r:id="rId31" display="https://leetcode.com/problems/rotting-oranges/" xr:uid="{15EA9BCE-06C4-4EEB-9796-6DABB67D400E}"/>
     <hyperlink ref="C35" r:id="rId32" display="https://leetcode.com/problems/pacific-atlantic-water-flow/" xr:uid="{A5087F08-C7AB-4992-B57F-A7D1AA6DD6C9}"/>
     <hyperlink ref="C36" r:id="rId33" display="https://leetcode.com/problems/surrounded-regions/" xr:uid="{2D073E62-CEDC-4D3A-9478-1237B343B174}"/>
+    <hyperlink ref="C38" r:id="rId34" display="https://leetcode.com/problems/course-schedule-ii/" xr:uid="{50EE1595-9B19-4FF7-BD0B-07B266F9F5F9}"/>
+    <hyperlink ref="C37" r:id="rId35" display="https://leetcode.com/problems/course-schedule/" xr:uid="{03F0A9F0-F706-4136-AAB3-D8670A47E565}"/>
+    <hyperlink ref="C39" r:id="rId36" xr:uid="{FD62D0F1-7F82-4A41-A089-7E5B5123B169}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 323 Number of Connected Components in an Undirected Graph - DFS
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{6BC2C32F-E44C-446C-A44E-0B3E03F1B9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFA78C88-DC04-4592-9325-BA395CBD987A}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{6BC2C32F-E44C-446C-A44E-0B3E03F1B9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{635FFBC7-5524-4C30-A0FC-A6F23E4FE966}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,9 +547,13 @@
     <t>261. Graph Valid Tree</t>
   </si>
   <si>
-    <t>Make a bi-directional adjacency matrix (WITH SETS) and add each edge and its inverse ((0, 1) and (1, 0))
-We'll do BFS so make a deque and a seen set for traversal and add 0 to both, then traverse LEVEL BY LEVEL and loop over curr nodes children and check if any of them are in seen (a cycle is found)
-Then add child to seen and remove curr from the child's neighbours set (adj[child]) (so we dont go back and do an infinite loop) return len(seen) == n to check if we have visited all nodes (unvisited/disconnected node means not a tree)</t>
+    <t>A valid tree must have exactly n - 1 edges and all nodes must be connected.
+Build a bi-directional adjacency list and use a queue of (node, parent) and a seen set starting from 0 for traversal
+Edge case: return False if len(edges) != n - 1 because in a valid tree, total edges are always 1 less than the total vertices
+For each neighbor:
+    - If it's already seen and not the parent, it means its a cycle so return False.
+    - Else mark it seen and push it to the queue as (child, curr).
+Finally, return len(seen) == n to check if we visited all nodes.</t>
   </si>
 </sst>
 </file>
@@ -960,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1504,7 +1508,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Solve Leetcode - 684. Redundant Connection - Union Find
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{6BC2C32F-E44C-446C-A44E-0B3E03F1B9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{635FFBC7-5524-4C30-A0FC-A6F23E4FE966}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1069E694-735C-49C1-B587-0A7FCCCCB766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="98">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -554,6 +554,34 @@
     - If it's already seen and not the parent, it means its a cycle so return False.
     - Else mark it seen and push it to the queue as (child, curr).
 Finally, return len(seen) == n to check if we visited all nodes.</t>
+  </si>
+  <si>
+    <t>Number of Connected Components in an Undirected Graph</t>
+  </si>
+  <si>
+    <t>We'll either use Union Find or DFS/BFS
+Start a DFS/BFS at every unvisited node; each start is one connected
+component, and the DFS just marks all nodes in that component as seen
+cycles don’t matter.
+Union-Find:
+- Initially, each node is its own parent (each node is its own component) and we also keep a "rank" array that stores the size of each component's root.
+- For every edge [a, b], we check if their roots are the same:
+        If yes → they're already in one component.
+        If no  → this edge connects two different components, so we merge them.
+- We merge smaller component into the bigger one (union by size) by attaching the smaller root to the bigger root and adding their sizes.
+- During find(), we apply path compression:
+        We recursively climb up until we find the root,
+        and along the way we set each node's parent directly to the root.
+    This flattens the structure, making all future finds extremely fast.</t>
+  </si>
+  <si>
+    <t>684. Redundant Connection</t>
+  </si>
+  <si>
+    <t>We'll use Union Find.
+The graph was initially a tree so each node WILL NOT have the same parent when we're building the tree otherwise there would be a cycle
+If two nodes have the same parent then connecting them would cause a cycle, and it would
+disqualify the tree property of the graph, so return the last one that causes a cycle</t>
   </si>
 </sst>
 </file>
@@ -693,10 +721,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -962,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1520,6 +1544,34 @@
       </c>
       <c r="D39" s="4" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1560,9 +1612,11 @@
     <hyperlink ref="C38" r:id="rId34" display="https://leetcode.com/problems/course-schedule-ii/" xr:uid="{50EE1595-9B19-4FF7-BD0B-07B266F9F5F9}"/>
     <hyperlink ref="C37" r:id="rId35" display="https://leetcode.com/problems/course-schedule/" xr:uid="{03F0A9F0-F706-4136-AAB3-D8670A47E565}"/>
     <hyperlink ref="C39" r:id="rId36" xr:uid="{FD62D0F1-7F82-4A41-A089-7E5B5123B169}"/>
+    <hyperlink ref="C40" r:id="rId37" xr:uid="{0B96D6C7-69AF-4248-BBA0-263A5C0C3AAE}"/>
+    <hyperlink ref="C41" r:id="rId38" display="https://leetcode.com/problems/redundant-connection/" xr:uid="{236C4B3B-429B-4D05-A987-BADF1F935248}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 743. Network Delay Time - Dijkstra's Algorithm
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Fullstack Dev Stuff\DSA\DSA-Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1069E694-735C-49C1-B587-0A7FCCCCB766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{1069E694-735C-49C1-B587-0A7FCCCCB766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D17DCA9-5FC3-4ED8-9F6D-7DC666E3C51F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="100">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -582,6 +582,16 @@
 The graph was initially a tree so each node WILL NOT have the same parent when we're building the tree otherwise there would be a cycle
 If two nodes have the same parent then connecting them would cause a cycle, and it would
 disqualify the tree property of the graph, so return the last one that causes a cycle</t>
+  </si>
+  <si>
+    <t>127. Word Ladder (!!!)</t>
+  </si>
+  <si>
+    <t>The core idea is to find the shortest path between two words by changing one letter at a time, making it a Breadth-First Search (BFS) problem. We can jump to any word as long as it differs by one letter, so that will be our graph, but to represent that optimally instead of the n^2 way of making adj list with a nested loop over all words + letters, we'll use the wildcard trick.
+To optimize, we use two key techniques:
+    1. Wildcard Pattern Trick to efficiently find neighbors by pre-processing the word list into an adjacency map (mapping patterns like "c*t" to all matching words like "cat", "cot", etc.)
+    2. Bi-directional BFS (Bi-BFS) starts searches simultaneously from both the beginWord and endWord and meets in the middle, exploring the smaller frontier at each step for massive performance gains, stopping when a word is found in the opposite frontier's visited set and returning the total level count.
+ The graph is pruned (adj[pattern] = []) after exploring a pattern's neighbors to avoid redundant work.</t>
   </si>
 </sst>
 </file>
@@ -986,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1572,6 +1582,20 @@
       </c>
       <c r="D41" s="4" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1614,9 +1638,10 @@
     <hyperlink ref="C39" r:id="rId36" xr:uid="{FD62D0F1-7F82-4A41-A089-7E5B5123B169}"/>
     <hyperlink ref="C40" r:id="rId37" xr:uid="{0B96D6C7-69AF-4248-BBA0-263A5C0C3AAE}"/>
     <hyperlink ref="C41" r:id="rId38" display="https://leetcode.com/problems/redundant-connection/" xr:uid="{236C4B3B-429B-4D05-A987-BADF1F935248}"/>
+    <hyperlink ref="C42" r:id="rId39" display="https://leetcode.com/problems/word-ladder/" xr:uid="{369F93BE-F82C-40E5-8F63-92B69F35DCBD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId39"/>
+  <pageSetup orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 787. Cheapest Flights Within K Stops - Dijkstra's + Hop Counting
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{1069E694-735C-49C1-B587-0A7FCCCCB766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D17DCA9-5FC3-4ED8-9F6D-7DC666E3C51F}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{1069E694-735C-49C1-B587-0A7FCCCCB766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE66FABF-6E25-467C-BBD5-3B5128A45117}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="112">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -592,6 +592,144 @@
     1. Wildcard Pattern Trick to efficiently find neighbors by pre-processing the word list into an adjacency map (mapping patterns like "c*t" to all matching words like "cat", "cot", etc.)
     2. Bi-directional BFS (Bi-BFS) starts searches simultaneously from both the beginWord and endWord and meets in the middle, exploring the smaller frontier at each step for massive performance gains, stopping when a word is found in the opposite frontier's visited set and returning the total level count.
  The graph is pruned (adj[pattern] = []) after exploring a pattern's neighbors to avoid redundant work.</t>
+  </si>
+  <si>
+    <t>Advanced Graphs</t>
+  </si>
+  <si>
+    <t>743. Network Delay Time</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">make an adj list then use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dijkstra's algo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Create a min heap and seen, heap will store the shortest path to n and have entries like (cost, node)
+Initialize heap with (0, k), then iterate while heap and pop the smallest item out of the heap, we first check if we've already seen it, 
+then that means that we have locked in its dist (since we always pop the shortest path to node N out of the heap, so if we're seeing it 
+again then that means shortest path has been locked in)
+For each node we pop, keep track of its cost with a res variable and keep updating it
+then add it to seen and iterate over its neighbours, and add those to the heap with (curDist + neighbourDist, neighbour) only if the neighbour
+is not in seen</t>
+    </r>
+  </si>
+  <si>
+    <t>332. Reconstruct Itinerary (!!!)</t>
+  </si>
+  <si>
+    <r>
+      <t>Euler Path/Hierholzer's Algo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. video - https://www.youtube.com/watch?v=5G0HyBhqpQo
+The problem statement states that at least one valid itinerary can be formed so we dont need to do the indegreee - outdegree calculation step to check if Euler path exists or not
+First we create an adjacency list but we sort tickets in descending lexical order before adding the edges, this is because Euler algo adds items from the end to start, and the problem statement states that the path with the smallest lexical order should be the answer
+Then we create a res list which will store the final positions of tickets and a stack, initialized with "JFK", which is where we'll add all items BEFORE we start popping any item and adding it to res 
+Then iterate as long as stack isnt empty, and for each airport we can go to from current airport, pop it from adj and add it to stack, mimicing a dfs, so go as deep as we can and once we're at the last airport and no more items are left in adj, then we'll add tickets from stack to res from the last airport all the way to first 
+Then reverse res and return</t>
+    </r>
+  </si>
+  <si>
+    <t>1584. Min Cost to Connect All Points</t>
+  </si>
+  <si>
+    <r>
+      <t>Prim's Alog (Optimized)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Since this is a connected graph and every vertex has an edge to every other vertex, we'll mantain weights and seen lists, both of size n
+Weights will be initialized with inf for all edges and seen will be False
+Start by adding any initial edge to weights with weight 0 and set seen for that node to True
+We'll iterate n times, one for each vertex, and in each loop we will select the minimum unseen weight, set it as seen and add its weight to total and then we'll update the dist for each node from this current node, for each unseen node, updating dist if its smaller
+and in the end return total</t>
+    </r>
+  </si>
+  <si>
+    <t>778. Swim in Rising Water</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dijkstra's Algo
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Start Dijkstra from top left, traverse in all directions, selecting shortest path and end when we hit bottm right.
+For distance, we'll just track the time/weight we need to traverse that particular neighbour by doing max(w, grid[nr][nc]) because
+we dont need to do culminative distance since the problem statement states that we can travel infinite distance as long as grid[i][j] &lt;= t
+So thats why we only need to return the max value of grid[i][j] we see in the shortest path from top left to bottom right</t>
+    </r>
+  </si>
+  <si>
+    <t>269. Alien Dictionary</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kahn's Topo Sort + Multi Source BFS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>We need to return the all the letters, and the letter whose relationship we do know should be in hierarchical order. Eg [ab, c], here we know that a is smaller than c so res will be "ac", but for b, we dont know since the comparison short circuited but we need to return all letters, so we can return "bac" or "abc", as long as a comes before c, the answer will be valid.
+That relationship gives us the idea that we're gonna need to maintain a graph/adjacency list to denote the relations. And whats a good algo for traversing stuff in some sort of hierarchy of relations, Topo Sort!
+We also notice that there could even be a forest possibly, e.g. ["ab", "bc", "rs", "tl"] forms three independent chains (a -&gt; b -&gt; c), (r -&gt; s), and (t -&gt; l), so the overall graph is a forest. So we'll use a multi source bfs
+Also there are 2 edge cases we need to consider -
+    Edge Case 1 - w1 is "abcd" and w2 is "abc", so there is no certain way to rank d and therefore according to constrains the list is invalid
+    Edge Case 2 - there is a cycle [ab, bc, ac] so this means a is less than b and b is also less than a, which is also not possible
+Start by initializing adj with a set and indegree with 0 for all letters (since what we return should have all letters)
+for each letter pair, first check for edge case 1 with the minLength match logic, then traverse them upto first non-matching character and then
+mark the relationship ONE TIME ([er, et, r, t] should not do indegree[t] for r 2 times) and then break immediately (since we cant conclude anything for letters after the first non-matching ones)
+Then just put all the items with indegree 0 into q, traverse the q until empty, then in the end we compare if topo sort procesed all elements (it
+wont if there is a cycle) by checking lengths and return the ans or "" for cycle</t>
+    </r>
+  </si>
+  <si>
+    <t>787. Cheapest Flights Within K Stops</t>
   </si>
 </sst>
 </file>
@@ -690,7 +828,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -712,6 +850,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -731,6 +870,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -996,15 +1139,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="115.44140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="115.44140625" customWidth="1"/>
@@ -1596,6 +1740,87 @@
       </c>
       <c r="D42" s="4" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="114" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1639,9 +1864,15 @@
     <hyperlink ref="C40" r:id="rId37" xr:uid="{0B96D6C7-69AF-4248-BBA0-263A5C0C3AAE}"/>
     <hyperlink ref="C41" r:id="rId38" display="https://leetcode.com/problems/redundant-connection/" xr:uid="{236C4B3B-429B-4D05-A987-BADF1F935248}"/>
     <hyperlink ref="C42" r:id="rId39" display="https://leetcode.com/problems/word-ladder/" xr:uid="{369F93BE-F82C-40E5-8F63-92B69F35DCBD}"/>
+    <hyperlink ref="C43" r:id="rId40" display="https://leetcode.com/problems/network-delay-time/" xr:uid="{16C353E0-ACB3-4FA5-8E89-2E50D9EAFE77}"/>
+    <hyperlink ref="C44" r:id="rId41" display="https://leetcode.com/problems/reconstruct-itinerary/" xr:uid="{43C4E869-CCE0-4E30-AD3D-231C374BE44E}"/>
+    <hyperlink ref="C45" r:id="rId42" display="https://leetcode.com/problems/min-cost-to-connect-all-points/" xr:uid="{57DD3173-42AC-45D1-9AF8-27B5C8D817CE}"/>
+    <hyperlink ref="C46" r:id="rId43" display="https://leetcode.com/problems/swim-in-rising-water/" xr:uid="{E6A62356-AC30-4F19-AB1D-810556084C4F}"/>
+    <hyperlink ref="C47" r:id="rId44" xr:uid="{35EA45D8-62A0-4E49-8C3C-910D7755AED0}"/>
+    <hyperlink ref="C48" r:id="rId45" display="https://leetcode.com/problems/cheapest-flights-within-k-stops/" xr:uid="{3D23E124-B1C7-4BDF-9D6D-2B2CF54683E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId46"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solve Leetcode - 70. Climbing Stairs - Bottom-Up DP (Fibonacci Optimization)
</commit_message>
<xml_diff>
--- a/Journal.xlsx
+++ b/Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f2b1b6a55c7a120/Desktop/Fullstack Dev Stuff/DSA/DSA-Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{1069E694-735C-49C1-B587-0A7FCCCCB766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE66FABF-6E25-467C-BBD5-3B5128A45117}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{1069E694-735C-49C1-B587-0A7FCCCCB766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36048B00-0FC4-4BD5-B990-289E91C0F362}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -730,6 +730,13 @@
   </si>
   <si>
     <t>787. Cheapest Flights Within K Stops</t>
+  </si>
+  <si>
+    <t>We'll use the Bellman Ford algorithm, with a little bit of customization (since there are no negative edges, but we do have egde hop limit)
+First initialize a list of prices for each node with inf for all edges except src which is 0
+Then for each hop, from i to k + 1 (k + 1 because if k = 0 we need to run the loop 1 time), update the price in a temp array for all the edges we can reach from current hop limit
+Skip any edge which is outside the current i hop limit by checking for prices[f] == inf
+Eg. for A -&gt; B, A -&gt; C, B -&gt; C, then for i == 0, we can process A -&gt; B and A -&gt; C but not B -&gt; C because that is 1 more hop so its prices[f] value will be inf to denote that, same for succeeding edges, but in the next i value, it will be accessible, change through prices being updated with temp</t>
   </si>
 </sst>
 </file>
@@ -828,7 +835,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -850,7 +857,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -1141,7 +1147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
@@ -1812,15 +1818,18 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>100</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="8" t="s">
         <v>111</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>